<commit_message>
Added state definitions to gorup products. Products in the same state for the same machine can be loaded without transition.
</commit_message>
<xml_diff>
--- a/input/scheduled_downtime.xlsx
+++ b/input/scheduled_downtime.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/karlahernandez/Desktop/STEM/supply_chain/dp-scheduling-wsetup/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{517ECAB0-513E-BB4D-803A-40A549A62B24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F632F91-34FE-EB4D-AD51-9D79202999B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="10360" yWindow="3120" windowWidth="28040" windowHeight="17440" xr2:uid="{7AF1CA2D-A986-AE48-8C82-95548A4C8927}"/>
   </bookViews>
@@ -36,10 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
-  <si>
-    <t>machine_Id</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>machine_1</t>
   </si>
@@ -54,6 +51,12 @@
   </si>
   <si>
     <t>machine_2</t>
+  </si>
+  <si>
+    <t>downtime_days</t>
+  </si>
+  <si>
+    <t>machine_id</t>
   </si>
 </sst>
 </file>
@@ -431,39 +434,47 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8860FFE-3274-D84F-ABA9-FC633046C2CD}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:B3"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="3" max="3" width="13.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B2" t="s">
         <v>2</v>
       </c>
+      <c r="C2">
+        <v>7</v>
+      </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" t="s">
-        <v>4</v>
+      <c r="C3">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>